<commit_message>
Adding the code for the raspberry pi to run
</commit_message>
<xml_diff>
--- a/Bill of Materials/Bill Of Materials.xlsx
+++ b/Bill of Materials/Bill Of Materials.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24923"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://berrycollege2-my.sharepoint.com/personal/colt_doster_vikings_berry_edu/Documents/CRT 499/OttoBot/Bill of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="11_F25DC773A252ABDACC1048DFF19A540E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39011008-1057-44B5-9D98-19EDEE5A22D6}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="11_F25DC773A252ABDACC1048DFF19A540E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D386D20-9E13-4FC5-8805-7FC0E60E1445}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Item</t>
   </si>
@@ -42,6 +51,9 @@
     <t>Link to purchase</t>
   </si>
   <si>
+    <t>Non-hardware Components</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raspberry Pi 3b+ </t>
   </si>
   <si>
@@ -60,27 +72,30 @@
     <t>https://www.amazon.com/Qunqi-Controller-Module-Stepper-Arduino/dp/B014KMHSW6/ref=asc_df_B014KMHSW6/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=167139094796&amp;hvpos=&amp;hvnetw=g&amp;hvrand=8134086289687349119&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9010853&amp;hvtargid=pla-306436938191&amp;psc=1</t>
   </si>
   <si>
+    <t>PCA9685 16 Channel 12 Bit PWM Servo Driver</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/SunFounder-PCA9685-Channel-Arduino-Raspberry/dp/B014KTSMLA/ref=sr_1_8?gclid=Cj0KCQiAip-PBhDVARIsAPP2xc3bwUdBIUvCkAtJKuVTAvXbtHdTCj0bSgghhUO9EcaGh_H8x-gnO0UaAhBzEALw_wcB&amp;hvadid=176344361500&amp;hvdev=c&amp;hvlocphy=9010853&amp;hvnetw=g&amp;hvqmt=e&amp;hvrand=8916339966619186825&amp;hvtargid=kwd-32310474982&amp;hydadcr=6241_9464970&amp;keywords=pca9685&amp;qid=1642606698&amp;sr=8-8</t>
   </si>
   <si>
-    <t>PCA9685 16 Channel 12 Bit PWM Servo Driver</t>
-  </si>
-  <si>
     <t xml:space="preserve">"Pi Power" Raspberry Pi power supply </t>
   </si>
   <si>
     <t>https://www.amazon.com/SunFounder-Raspberry-Recharging-Function-Expansion/dp/B08HLXGS3W/ref=sr_1_3?crid=3QI7CPQCM0RPB&amp;keywords=Sunfounder+pi+power&amp;qid=1642606946&amp;sprefix=sunfounder+pi+powe%2Caps%2C81&amp;sr=8-3</t>
   </si>
   <si>
+    <t>DC Motors w/wheels (2pack)</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/Stemedu-Gearbox-Motor-200RPM-Arduino/dp/B07L881GXZ/ref=sr_1_8?keywords=DC+Motor+Wheel&amp;qid=1642607082&amp;sr=8-8</t>
   </si>
   <si>
-    <t>DC Motors w/wheels (2pack)</t>
-  </si>
-  <si>
     <t>Non-active front wheels (at least 2 pack)</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B01MXDCQ1F/ref=sspa_dk_detail_7?psc=1&amp;pd_rd_i=B01MXDCQ1F&amp;pd_rd_w=nJ9Id&amp;pf_rd_p=887084a2-5c34-4113-a4f8-b7947847c308&amp;pd_rd_wg=LAa4m&amp;pf_rd_r=A9CDCGWXS5JRSF694HEB&amp;pd_rd_r=1f9721d6-1fff-46d8-a162-9a2fa7c6fd0e&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyOTFDWDhERTY5MTNFJmVuY3J5cHRlZElkPUExMDQ4MDQ1NVVOM1NRQUgwSUIwJmVuY3J5cHRlZEFkSWQ9QTA3Mzc2ODY4NjU5RUVEOE5JMTkmd2lkZ2V0TmFtZT1zcF9kZXRhaWwmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl </t>
+  </si>
+  <si>
     <t xml:space="preserve">2 slot 18650 battery holder </t>
   </si>
   <si>
@@ -111,7 +126,10 @@
     <t>https://www.amazon.com/dp/B09QQDRDCL/ref=sr_1_2_sspa?gclid=Cj0KCQiAip-PBhDVARIsAPP2xc0YcnnJz-HEaBY8mhcu2Dm-tAmfBkLcv0eyF48J16aaq2ORdLtrMO8aAtTREALw_wcB&amp;hvadid=416723314767&amp;hvdev=c&amp;hvlocphy=9010853&amp;hvnetw=g&amp;hvqmt=e&amp;hvrand=12598012965231412216&amp;hvtargid=kwd-378448531677&amp;hydadcr=19103_11276217&amp;keywords=18650-battery&amp;qid=1642608447&amp;s=electronics&amp;sr=1-2-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUE2MDhJNUdJTkdMRzAmZW5jcnlwdGVkSWQ9QTAwODc4NTAySVdIM1EyUjExV01OJmVuY3J5cHRlZEFkSWQ9QTA4OTg4MzNOOThVMFJERU42R04md2lkZ2V0TmFtZT1zcF9hdGYmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl</t>
   </si>
   <si>
-    <t>Non-hardware Components</t>
+    <t>Acrylic Sheet</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SimbaLux-Plexiglass-Transparent-Protective-Projects/dp/B07RY4X9L3/ref=sr_1_3?gclid=Cj0KCQiAip-PBhDVARIsAPP2xc1piLtEpcIR4uXfFe1FGuzlbOCr7IZ4_x6QXH3NAFoEEPUbdXYTyKsaAg-MEALw_wcB&amp;hvadid=174244429573&amp;hvdev=c&amp;hvlocphy=9010853&amp;hvnetw=g&amp;hvqmt=e&amp;hvrand=4231034287874400623&amp;hvtargid=kwd-68751927087&amp;hydadcr=24658_9648989&amp;keywords=1%2F8+acrylic+sheet&amp;qid=1642627760&amp;sr=8-3</t>
   </si>
   <si>
     <t>Hardware Compnents</t>
@@ -156,15 +174,15 @@
     <t>M 3 x24 standoffs</t>
   </si>
   <si>
-    <t xml:space="preserve">CANNOT FIND </t>
+    <t>https://www.amazon.com/jing-Standoff-Quadcopter-Computer-Circuit/dp/B0975SLD2K/ref=sr_1_1_sspa?keywords=M3+x+25+standoff&amp;qid=1643141993&amp;s=industrial&amp;sr=1-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExQkg1MUNCTk9GWENHJmVuY3J5cHRlZElkPUEwNTU3MzkxMUpJUDBXM0E2SE9YOSZlbmNyeXB0ZWRBZElkPUEwOTkwNzE1MkoxVTFFUkxGVUFHOSZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=</t>
+  </si>
+  <si>
+    <t>M2 nuts (sold in larger pack)</t>
   </si>
   <si>
     <t>https://www.amazon.com/uxcell-Metric-Stainless-Hexagon-Silver/dp/B07H3SXSN2/ref=sr_1_3?crid=3OFQXA7OTQZIQ&amp;keywords=m2+nuts&amp;qid=1642610731&amp;s=industrial&amp;sprefix=m2+nuts%2Cindustrial%2C69&amp;sr=1-3</t>
   </si>
   <si>
-    <t>M2 nuts (sold in larger pack)</t>
-  </si>
-  <si>
     <t>M2.5 nuts (sold in larger pack)</t>
   </si>
   <si>
@@ -177,25 +195,19 @@
     <t>https://www.amazon.com/Shapenty-100PCS-Stainless-Female-Fastener/dp/B071NLDW56/ref=sr_1_4?crid=215UETHAFDZ4E&amp;keywords=m3+nuts&amp;qid=1642626855&amp;s=industrial&amp;sprefix=m3+nuts%2Cindustrial%2C75&amp;sr=1-4</t>
   </si>
   <si>
+    <t>M4 self locking nuts (sold in larger pack)</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/Fullerkreg-Self-Locking-Stainless-18-8%EF%BC%8CPlain-Quantity/dp/B078T4V7WZ/ref=sr_1_1_sspa?crid=1XABXO88L4QF5&amp;keywords=m4+self+locking+nut&amp;qid=1642626969&amp;sprefix=M4+self+lo%2Caps%2C77&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyN1VJRURXV0FWS045JmVuY3J5cHRlZElkPUEwMTAzMjI2VEtYWE03SldMVzNEJmVuY3J5cHRlZEFkSWQ9QTA0NjIzNzExWEczMFYxQjJCRTdaJndpZGdldE5hbWU9c3BfYXRmJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==</t>
   </si>
   <si>
-    <t>M4 self locking nuts (sold in larger pack)</t>
-  </si>
-  <si>
     <t>F694ZZ wheel bearings (2 pack)</t>
   </si>
   <si>
     <t>https://www.amazon.com/Othmro-Groove-Bearing-4x11x12-5x4x1mm-Bearings/dp/B082SNKSN7/ref=sr_1_6?crid=AACO6JI7NUHU&amp;keywords=f694zz&amp;qid=1642627466&amp;sprefix=F694zz%2Caps%2C167&amp;sr=8-6</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B01MXDCQ1F/ref=sspa_dk_detail_7?psc=1&amp;pd_rd_i=B01MXDCQ1F&amp;pd_rd_w=nJ9Id&amp;pf_rd_p=887084a2-5c34-4113-a4f8-b7947847c308&amp;pd_rd_wg=LAa4m&amp;pf_rd_r=A9CDCGWXS5JRSF694HEB&amp;pd_rd_r=1f9721d6-1fff-46d8-a162-9a2fa7c6fd0e&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyOTFDWDhERTY5MTNFJmVuY3J5cHRlZElkPUExMDQ4MDQ1NVVOM1NRQUgwSUIwJmVuY3J5cHRlZEFkSWQ9QTA3Mzc2ODY4NjU5RUVEOE5JMTkmd2lkZ2V0TmFtZT1zcF9kZXRhaWwmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl </t>
-  </si>
-  <si>
-    <t>Acrylic Sheet</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/SimbaLux-Plexiglass-Transparent-Protective-Projects/dp/B07RY4X9L3/ref=sr_1_3?gclid=Cj0KCQiAip-PBhDVARIsAPP2xc1piLtEpcIR4uXfFe1FGuzlbOCr7IZ4_x6QXH3NAFoEEPUbdXYTyKsaAg-MEALw_wcB&amp;hvadid=174244429573&amp;hvdev=c&amp;hvlocphy=9010853&amp;hvnetw=g&amp;hvqmt=e&amp;hvrand=4231034287874400623&amp;hvtargid=kwd-68751927087&amp;hydadcr=24658_9648989&amp;keywords=1%2F8+acrylic+sheet&amp;qid=1642627760&amp;sr=8-3</t>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -205,7 +217,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,22 +569,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="52.88671875" customWidth="1"/>
+    <col min="1" max="1" width="47.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,14 +601,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -608,12 +620,12 @@
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -625,12 +637,12 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -642,10 +654,10 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -659,12 +671,12 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -676,10 +688,10 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -693,12 +705,12 @@
         <v>10</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -710,12 +722,12 @@
         <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -727,12 +739,12 @@
         <v>8</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -744,12 +756,12 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -761,12 +773,12 @@
         <v>10</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -778,12 +790,12 @@
         <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -795,12 +807,12 @@
         <v>20</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -812,17 +824,17 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -834,12 +846,12 @@
         <v>14</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -851,12 +863,12 @@
         <v>7</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -868,12 +880,12 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -885,12 +897,12 @@
         <v>30</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -902,12 +914,12 @@
         <v>0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -919,12 +931,12 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -936,23 +948,29 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="2">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -964,12 +982,12 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -981,12 +999,12 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -998,12 +1016,12 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1015,12 +1033,12 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1032,7 +1050,16 @@
         <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4">
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="2">
+        <f>SUM(D4:D31)</f>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -1047,8 +1074,9 @@
     <hyperlink ref="E22" r:id="rId8" display="https://www.amazon.com/iExcell-Thread-Stainless-Washers-Assortment/dp/B08LQDLV51/ref=sr_1_1_sspa?crid=1LKAUD20MI7OV&amp;keywords=m3%2Bscrew%2Bkit&amp;qid=1642609215&amp;s=industrial&amp;sprefix=m3%2Bscrew%2Bkit%2Cindustrial%2C63&amp;sr=1-1-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyU0xQVU8wQU0zVUlHJmVuY3J5cHRlZElkPUExMDM5MjU5MzVIUTZWWDZTOVdDTSZlbmNyeXB0ZWRBZElkPUEwNDg0OTA0MUdUWUI1NFNCOUhUTyZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU&amp;th=1" xr:uid="{BC6ACDD0-66ED-4035-A017-D7CC5440098C}"/>
     <hyperlink ref="E23" r:id="rId9" display="https://www.amazon.com/iExcell-Thread-Stainless-Washers-Assortment/dp/B08LQDLV51/ref=sr_1_1_sspa?crid=1LKAUD20MI7OV&amp;keywords=m3%2Bscrew%2Bkit&amp;qid=1642609215&amp;s=industrial&amp;sprefix=m3%2Bscrew%2Bkit%2Cindustrial%2C63&amp;sr=1-1-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyU0xQVU8wQU0zVUlHJmVuY3J5cHRlZElkPUExMDM5MjU5MzVIUTZWWDZTOVdDTSZlbmNyeXB0ZWRBZElkPUEwNDg0OTA0MUdUWUI1NFNCOUhUTyZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU&amp;th=1" xr:uid="{15A9E498-EBBB-4384-9609-68F5A6BEF562}"/>
     <hyperlink ref="E10" r:id="rId10" display="https://www.amazon.com/dp/B01MXDCQ1F/ref=sspa_dk_detail_7?psc=1&amp;pd_rd_i=B01MXDCQ1F&amp;pd_rd_w=nJ9Id&amp;pf_rd_p=887084a2-5c34-4113-a4f8-b7947847c308&amp;pd_rd_wg=LAa4m&amp;pf_rd_r=A9CDCGWXS5JRSF694HEB&amp;pd_rd_r=1f9721d6-1fff-46d8-a162-9a2fa7c6fd0e&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyOTFDWDhERTY5MTNFJmVuY3J5cHRlZElkPUExMDQ4MDQ1NVVOM1NRQUgwSUIwJmVuY3J5cHRlZEFkSWQ9QTA3Mzc2ODY4NjU5RUVEOE5JMTkmd2lkZ2V0TmFtZT1zcF9kZXRhaWwmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl " xr:uid="{0576796F-9430-4E7F-AE3A-8AE336FC44DB}"/>
+    <hyperlink ref="E26" r:id="rId11" display="https://www.amazon.com/jing-Standoff-Quadcopter-Computer-Circuit/dp/B0975SLD2K/ref=sr_1_1_sspa?keywords=M3+x+25+standoff&amp;qid=1643141993&amp;s=industrial&amp;sr=1-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExQkg1MUNCTk9GWENHJmVuY3J5cHRlZElkPUEwNTU3MzkxMUpJUDBXM0E2SE9YOSZlbmNyeXB0ZWRBZElkPUEwOTkwNzE1MkoxVTFFUkxGVUFHOSZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{D6F33DD7-4554-42BD-8B20-EF246A061E53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>